<commit_message>
Revert "Merge branch 'main' of https://github.com/Wowo567/Wowo666"
This reverts commit b0582508eb4d02174421158ac3404c9a7ee1e2fe, reversing
changes made to 29af94c173131f1b973bf82c30b2b2ac666290eb.
</commit_message>
<xml_diff>
--- a/Global Game Jam 2025/Assets/Datas/ComicItemDatas.xlsx
+++ b/Global Game Jam 2025/Assets/Datas/ComicItemDatas.xlsx
@@ -37,13 +37,13 @@
     <t>ComicItem_1-2</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>ComicItem_1-3</t>
   </si>
   <si>
     <t>ComicItem_1-4</t>
+  </si>
+  <si>
+    <t>ComicItem_0-1</t>
   </si>
 </sst>
 </file>
@@ -998,13 +998,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="F1" sqref="F$1:F$1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="20.5961538461538" customWidth="1"/>
     <col min="3" max="3" width="15.9038461538462" customWidth="1"/>
@@ -1039,7 +1039,9 @@
       <c r="C2" s="1">
         <v>12</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
@@ -1054,8 +1056,8 @@
       <c r="C3" s="1">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="D3" s="1">
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -1066,7 +1068,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>14</v>
@@ -1083,15 +1085,51 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
+    </row>
+    <row r="6" ht="17.6" spans="1:6">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" ht="17.6" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" ht="17.6" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:G4">

</xml_diff>